<commit_message>
Added Support for ShopOrderAgent WorkCenterAgent communication: single instance: only one operation will be communicated to the work center agent Added util classes and method. Basic code refactoring
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="ShopOrders" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
   <si>
     <t>OrderNo</t>
   </si>
@@ -124,12 +124,6 @@
   </si>
   <si>
     <t>op1</t>
-  </si>
-  <si>
-    <t>op2</t>
-  </si>
-  <si>
-    <t>op3</t>
   </si>
   <si>
     <t>WorkCenterType</t>
@@ -517,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +584,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="1">
-        <v>43310</v>
+        <v>43318</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>15</v>
@@ -628,10 +622,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,16 +641,17 @@
     <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>21</v>
@@ -689,13 +684,16 @@
         <v>30</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -721,73 +719,9 @@
         <v>2</v>
       </c>
       <c r="M2" t="s">
-        <v>38</v>
-      </c>
-      <c r="N2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>8</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>10</v>
-      </c>
-      <c r="M3" t="s">
-        <v>42</v>
-      </c>
-      <c r="N3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>30</v>
-      </c>
-      <c r="D4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>4</v>
-      </c>
-      <c r="M4" t="s">
-        <v>38</v>
-      </c>
-      <c r="N4" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -802,7 +736,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,41 +752,41 @@
         <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
         <v>38</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -864,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,42 +813,42 @@
         <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>45</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>46</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>47</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>49</v>
-      </c>
-      <c r="I1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1">
         <v>43318</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I2">
         <v>3</v>
@@ -922,7 +856,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3" s="1">
         <v>43319</v>
@@ -936,7 +870,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" s="1">
         <v>43320</v>
@@ -950,7 +884,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="1">
         <v>43321</v>
@@ -961,7 +895,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1">
         <v>43322</v>
@@ -969,7 +903,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B7" s="1">
         <v>43323</v>
@@ -977,7 +911,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1">
         <v>43324</v>
@@ -991,7 +925,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B9" s="1">
         <v>43318</v>
@@ -999,7 +933,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1">
         <v>43319</v>
@@ -1010,7 +944,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1">
         <v>43320</v>
@@ -1021,7 +955,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1">
         <v>43321</v>
@@ -1035,7 +969,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B13" s="1">
         <v>43322</v>
@@ -1046,7 +980,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" s="1">
         <v>43323</v>
@@ -1057,7 +991,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1">
         <v>43324</v>

</xml_diff>

<commit_message>
DateTime Comparison support: now includes time comparsion
Added better support for Date Comparison
Included Joda Time library for DateTIme manipulation work
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ShopOrders" sheetId="1" r:id="rId1"/>
@@ -511,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
DYNO-02: Best offer should be updated on the DB
Handled updating the excel file and add the OperationId on the respective TimeBlock and the date
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ShopOrders" sheetId="1" r:id="rId1"/>
@@ -512,24 +512,24 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="4" width="14.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" customWidth="1"/>
-    <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" customWidth="1"/>
-    <col min="13" max="13" width="17.140625" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="14.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -624,26 +624,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -741,10 +741,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -798,14 +798,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -930,6 +930,9 @@
       <c r="B9" s="1">
         <v>43318</v>
       </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">

</xml_diff>